<commit_message>
adding time series changes
</commit_message>
<xml_diff>
--- a/data/Specifications_mfvar.xlsx
+++ b/data/Specifications_mfvar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\Boris_MF_VAR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boris\Dropbox\JuliaNew\BEAVARs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F656B091-128E-471B-9349-4ECABF19C9E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754C5D96-668A-48B3-AE77-6922F818795D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="explanation" sheetId="2" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="142">
   <si>
     <t>FullNames</t>
   </si>
@@ -497,6 +497,12 @@
   <si>
     <t>survConsBG</t>
   </si>
+  <si>
+    <t>bg_jul</t>
+  </si>
+  <si>
+    <t>bg_julL</t>
+  </si>
 </sst>
 </file>
 
@@ -14749,7 +14755,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23572,14 +23578,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA007589-EAEC-4D00-B420-95C3C7F78D53}">
-  <dimension ref="A1:Y93"/>
+  <dimension ref="A1:W72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E42" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E20" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F2" sqref="F2"/>
       <selection pane="topRight" activeCell="F2" sqref="F2"/>
       <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
-      <selection pane="bottomRight" activeCell="A58" sqref="A58:XFD58"/>
+      <selection pane="bottomRight" activeCell="T7" sqref="T6:T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23592,7 +23598,7 @@
     <col min="15" max="20" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -23656,12 +23662,14 @@
       <c r="U1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -23725,12 +23733,14 @@
       <c r="U2" s="10">
         <v>0</v>
       </c>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="10"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V2" s="10">
+        <v>0</v>
+      </c>
+      <c r="W2" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>22</v>
       </c>
@@ -23794,12 +23804,14 @@
       <c r="U3" s="18">
         <v>10</v>
       </c>
-      <c r="V3" s="18"/>
-      <c r="W3" s="18"/>
-      <c r="X3" s="18"/>
-      <c r="Y3" s="18"/>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V3" s="18">
+        <v>10</v>
+      </c>
+      <c r="W3" s="18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>32</v>
       </c>
@@ -23863,12 +23875,14 @@
       <c r="U4" s="18">
         <v>0</v>
       </c>
-      <c r="V4" s="18"/>
-      <c r="W4" s="18"/>
-      <c r="X4" s="18"/>
-      <c r="Y4" s="18"/>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V4" s="18">
+        <v>0</v>
+      </c>
+      <c r="W4" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>33</v>
       </c>
@@ -23932,12 +23946,14 @@
       <c r="U5" s="18">
         <v>0</v>
       </c>
-      <c r="V5" s="18"/>
-      <c r="W5" s="18"/>
-      <c r="X5" s="18"/>
-      <c r="Y5" s="18"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V5" s="18">
+        <v>0</v>
+      </c>
+      <c r="W5" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>34</v>
       </c>
@@ -24001,12 +24017,14 @@
       <c r="U6" s="18">
         <v>0</v>
       </c>
-      <c r="V6" s="18"/>
-      <c r="W6" s="18"/>
-      <c r="X6" s="18"/>
-      <c r="Y6" s="18"/>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V6" s="18">
+        <v>0</v>
+      </c>
+      <c r="W6" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>35</v>
       </c>
@@ -24070,12 +24088,14 @@
       <c r="U7" s="18">
         <v>0</v>
       </c>
-      <c r="V7" s="18"/>
-      <c r="W7" s="18"/>
-      <c r="X7" s="18"/>
-      <c r="Y7" s="18"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V7" s="18">
+        <v>0</v>
+      </c>
+      <c r="W7" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>23</v>
       </c>
@@ -24139,12 +24159,14 @@
       <c r="U8" s="25">
         <v>1</v>
       </c>
-      <c r="V8" s="25"/>
-      <c r="W8" s="25"/>
-      <c r="X8" s="25"/>
-      <c r="Y8" s="25"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V8" s="25">
+        <v>1</v>
+      </c>
+      <c r="W8" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>24</v>
       </c>
@@ -24208,12 +24230,14 @@
       <c r="U9" s="25">
         <v>2005</v>
       </c>
-      <c r="V9" s="25"/>
-      <c r="W9" s="25"/>
-      <c r="X9" s="25"/>
-      <c r="Y9" s="25"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V9" s="25">
+        <v>2005</v>
+      </c>
+      <c r="W9" s="25">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>25</v>
       </c>
@@ -24277,12 +24301,14 @@
       <c r="U10" s="18">
         <v>0</v>
       </c>
-      <c r="V10" s="18"/>
-      <c r="W10" s="18"/>
-      <c r="X10" s="18"/>
-      <c r="Y10" s="18"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V10" s="18">
+        <v>0</v>
+      </c>
+      <c r="W10" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>26</v>
       </c>
@@ -24346,12 +24372,14 @@
       <c r="U11" s="18">
         <v>0</v>
       </c>
-      <c r="V11" s="18"/>
-      <c r="W11" s="18"/>
-      <c r="X11" s="18"/>
-      <c r="Y11" s="18"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V11" s="18">
+        <v>0</v>
+      </c>
+      <c r="W11" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>120</v>
       </c>
@@ -24415,12 +24443,14 @@
       <c r="U12" s="18">
         <v>0</v>
       </c>
-      <c r="V12" s="18"/>
-      <c r="W12" s="18"/>
-      <c r="X12" s="18"/>
-      <c r="Y12" s="18"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V12" s="18">
+        <v>0</v>
+      </c>
+      <c r="W12" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>119</v>
       </c>
@@ -24484,12 +24514,14 @@
       <c r="U13" s="18">
         <v>0</v>
       </c>
-      <c r="V13" s="18"/>
-      <c r="W13" s="18"/>
-      <c r="X13" s="18"/>
-      <c r="Y13" s="18"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V13" s="18">
+        <v>0</v>
+      </c>
+      <c r="W13" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>27</v>
       </c>
@@ -24553,12 +24585,14 @@
       <c r="U14" s="18">
         <v>0</v>
       </c>
-      <c r="V14" s="18"/>
-      <c r="W14" s="18"/>
-      <c r="X14" s="18"/>
-      <c r="Y14" s="18"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V14" s="18">
+        <v>0</v>
+      </c>
+      <c r="W14" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>3</v>
       </c>
@@ -24622,12 +24656,14 @@
       <c r="U15" s="10">
         <v>0</v>
       </c>
-      <c r="V15" s="10"/>
-      <c r="W15" s="10"/>
-      <c r="X15" s="10"/>
-      <c r="Y15" s="10"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V15" s="10">
+        <v>0</v>
+      </c>
+      <c r="W15" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>4</v>
       </c>
@@ -24691,12 +24727,14 @@
       <c r="U16" s="10">
         <v>0</v>
       </c>
-      <c r="V16" s="10"/>
-      <c r="W16" s="10"/>
-      <c r="X16" s="10"/>
-      <c r="Y16" s="10"/>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V16" s="10">
+        <v>0</v>
+      </c>
+      <c r="W16" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>5</v>
       </c>
@@ -24760,12 +24798,14 @@
       <c r="U17" s="10">
         <v>6</v>
       </c>
-      <c r="V17" s="10"/>
-      <c r="W17" s="10"/>
-      <c r="X17" s="10"/>
-      <c r="Y17" s="10"/>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V17" s="10">
+        <v>6</v>
+      </c>
+      <c r="W17" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>6</v>
       </c>
@@ -24829,12 +24869,14 @@
       <c r="U18" s="10">
         <v>12</v>
       </c>
-      <c r="V18" s="10"/>
-      <c r="W18" s="10"/>
-      <c r="X18" s="10"/>
-      <c r="Y18" s="10"/>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V18" s="10">
+        <v>12</v>
+      </c>
+      <c r="W18" s="10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>28</v>
       </c>
@@ -24898,12 +24940,14 @@
       <c r="U19" s="10">
         <v>1</v>
       </c>
-      <c r="V19" s="10"/>
-      <c r="W19" s="10"/>
-      <c r="X19" s="10"/>
-      <c r="Y19" s="10"/>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V19" s="10">
+        <v>2</v>
+      </c>
+      <c r="W19" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>36</v>
       </c>
@@ -24967,12 +25011,14 @@
       <c r="U20" s="18">
         <v>1</v>
       </c>
-      <c r="V20" s="18"/>
-      <c r="W20" s="18"/>
-      <c r="X20" s="18"/>
-      <c r="Y20" s="18"/>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V20" s="18">
+        <v>1</v>
+      </c>
+      <c r="W20" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>37</v>
       </c>
@@ -25036,12 +25082,14 @@
       <c r="U21" s="18">
         <v>2</v>
       </c>
-      <c r="V21" s="18"/>
-      <c r="W21" s="18"/>
-      <c r="X21" s="18"/>
-      <c r="Y21" s="18"/>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V21" s="18">
+        <v>2</v>
+      </c>
+      <c r="W21" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>29</v>
       </c>
@@ -25105,12 +25153,14 @@
       <c r="U22" s="10">
         <v>5</v>
       </c>
-      <c r="V22" s="10"/>
-      <c r="W22" s="10"/>
-      <c r="X22" s="10"/>
-      <c r="Y22" s="10"/>
-    </row>
-    <row r="23" spans="1:25" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="V22" s="10">
+        <v>5</v>
+      </c>
+      <c r="W22" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>9</v>
       </c>
@@ -25174,12 +25224,14 @@
       <c r="U23" s="11">
         <v>20000</v>
       </c>
-      <c r="V23" s="11"/>
-      <c r="W23" s="11"/>
-      <c r="X23" s="11"/>
-      <c r="Y23" s="11"/>
-    </row>
-    <row r="24" spans="1:25" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="V23" s="11">
+        <v>5000</v>
+      </c>
+      <c r="W23" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>8</v>
       </c>
@@ -25243,12 +25295,14 @@
       <c r="U24" s="11">
         <v>10000</v>
       </c>
-      <c r="V24" s="11"/>
-      <c r="W24" s="11"/>
-      <c r="X24" s="11"/>
-      <c r="Y24" s="11"/>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V24" s="11">
+        <v>5000</v>
+      </c>
+      <c r="W24" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>10</v>
       </c>
@@ -25312,12 +25366,14 @@
       <c r="U25" s="11">
         <v>1</v>
       </c>
-      <c r="V25" s="11"/>
-      <c r="W25" s="11"/>
-      <c r="X25" s="11"/>
-      <c r="Y25" s="11"/>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V25" s="11">
+        <v>1</v>
+      </c>
+      <c r="W25" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>31</v>
       </c>
@@ -25381,12 +25437,14 @@
       <c r="U26" s="11">
         <v>0</v>
       </c>
-      <c r="V26" s="11"/>
-      <c r="W26" s="11"/>
-      <c r="X26" s="11"/>
-      <c r="Y26" s="11"/>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V26" s="11">
+        <v>0</v>
+      </c>
+      <c r="W26" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>30</v>
       </c>
@@ -25450,12 +25508,14 @@
       <c r="U27" s="11">
         <v>1</v>
       </c>
-      <c r="V27" s="11"/>
-      <c r="W27" s="11"/>
-      <c r="X27" s="11"/>
-      <c r="Y27" s="11"/>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V27" s="11">
+        <v>1</v>
+      </c>
+      <c r="W27" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>7</v>
       </c>
@@ -25519,12 +25579,14 @@
       <c r="U28" s="11">
         <v>4</v>
       </c>
-      <c r="V28" s="11"/>
-      <c r="W28" s="11"/>
-      <c r="X28" s="11"/>
-      <c r="Y28" s="11"/>
-    </row>
-    <row r="29" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="V28" s="11">
+        <v>4</v>
+      </c>
+      <c r="W28" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>11</v>
       </c>
@@ -25588,12 +25650,14 @@
       <c r="U29" s="12">
         <v>12</v>
       </c>
-      <c r="V29" s="12"/>
-      <c r="W29" s="12"/>
-      <c r="X29" s="12"/>
-      <c r="Y29" s="12"/>
-    </row>
-    <row r="30" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="V29" s="12">
+        <v>12</v>
+      </c>
+      <c r="W29" s="12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>38</v>
       </c>
@@ -25657,12 +25721,14 @@
       <c r="U30" s="14">
         <v>0</v>
       </c>
-      <c r="V30" s="14"/>
-      <c r="W30" s="14"/>
-      <c r="X30" s="14"/>
-      <c r="Y30" s="14"/>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V30" s="14">
+        <v>0</v>
+      </c>
+      <c r="W30" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>76</v>
       </c>
@@ -25726,12 +25792,14 @@
       <c r="U31" s="13">
         <v>0</v>
       </c>
-      <c r="V31" s="13"/>
-      <c r="W31" s="13"/>
-      <c r="X31" s="13"/>
-      <c r="Y31" s="13"/>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V31" s="13">
+        <v>0</v>
+      </c>
+      <c r="W31" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -25795,12 +25863,14 @@
       <c r="U32" s="13">
         <v>0</v>
       </c>
-      <c r="V32" s="13"/>
-      <c r="W32" s="13"/>
-      <c r="X32" s="13"/>
-      <c r="Y32" s="13"/>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V32" s="13">
+        <v>0</v>
+      </c>
+      <c r="W32" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -25864,12 +25934,14 @@
       <c r="U33" s="13">
         <v>0</v>
       </c>
-      <c r="V33" s="13"/>
-      <c r="W33" s="13"/>
-      <c r="X33" s="13"/>
-      <c r="Y33" s="13"/>
-    </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V33" s="13">
+        <v>0</v>
+      </c>
+      <c r="W33" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>67</v>
       </c>
@@ -25933,12 +26005,14 @@
       <c r="U34" s="13">
         <v>0</v>
       </c>
-      <c r="V34" s="13"/>
-      <c r="W34" s="13"/>
-      <c r="X34" s="13"/>
-      <c r="Y34" s="13"/>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V34" s="13">
+        <v>0</v>
+      </c>
+      <c r="W34" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -26002,12 +26076,14 @@
       <c r="U35" s="13">
         <v>0</v>
       </c>
-      <c r="V35" s="13"/>
-      <c r="W35" s="13"/>
-      <c r="X35" s="13"/>
-      <c r="Y35" s="13"/>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V35" s="13">
+        <v>0</v>
+      </c>
+      <c r="W35" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -26071,12 +26147,14 @@
       <c r="U36" s="13">
         <v>0</v>
       </c>
-      <c r="V36" s="13"/>
-      <c r="W36" s="13"/>
-      <c r="X36" s="13"/>
-      <c r="Y36" s="13"/>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V36" s="13">
+        <v>0</v>
+      </c>
+      <c r="W36" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -26140,12 +26218,14 @@
       <c r="U37" s="13">
         <v>0</v>
       </c>
-      <c r="V37" s="13"/>
-      <c r="W37" s="13"/>
-      <c r="X37" s="13"/>
-      <c r="Y37" s="13"/>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V37" s="13">
+        <v>0</v>
+      </c>
+      <c r="W37" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>69</v>
       </c>
@@ -26209,12 +26289,14 @@
       <c r="U38" s="13">
         <v>0</v>
       </c>
-      <c r="V38" s="13"/>
-      <c r="W38" s="13"/>
-      <c r="X38" s="13"/>
-      <c r="Y38" s="13"/>
-    </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V38" s="13">
+        <v>0</v>
+      </c>
+      <c r="W38" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>70</v>
       </c>
@@ -26278,12 +26360,14 @@
       <c r="U39" s="13">
         <v>0</v>
       </c>
-      <c r="V39" s="13"/>
-      <c r="W39" s="13"/>
-      <c r="X39" s="13"/>
-      <c r="Y39" s="13"/>
-    </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V39" s="13">
+        <v>0</v>
+      </c>
+      <c r="W39" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>15</v>
       </c>
@@ -26347,12 +26431,14 @@
       <c r="U40" s="13">
         <v>0</v>
       </c>
-      <c r="V40" s="13"/>
-      <c r="W40" s="13"/>
-      <c r="X40" s="13"/>
-      <c r="Y40" s="13"/>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V40" s="13">
+        <v>0</v>
+      </c>
+      <c r="W40" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>71</v>
       </c>
@@ -26416,12 +26502,14 @@
       <c r="U41" s="13">
         <v>0</v>
       </c>
-      <c r="V41" s="13"/>
-      <c r="W41" s="13"/>
-      <c r="X41" s="13"/>
-      <c r="Y41" s="13"/>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V41" s="13">
+        <v>0</v>
+      </c>
+      <c r="W41" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>72</v>
       </c>
@@ -26485,12 +26573,14 @@
       <c r="U42" s="13">
         <v>0</v>
       </c>
-      <c r="V42" s="13"/>
-      <c r="W42" s="13"/>
-      <c r="X42" s="13"/>
-      <c r="Y42" s="13"/>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V42" s="13">
+        <v>0</v>
+      </c>
+      <c r="W42" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -26554,12 +26644,14 @@
       <c r="U43" s="13">
         <v>0</v>
       </c>
-      <c r="V43" s="13"/>
-      <c r="W43" s="13"/>
-      <c r="X43" s="13"/>
-      <c r="Y43" s="13"/>
-    </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V43" s="13">
+        <v>0</v>
+      </c>
+      <c r="W43" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>73</v>
       </c>
@@ -26623,12 +26715,14 @@
       <c r="U44" s="13">
         <v>0</v>
       </c>
-      <c r="V44" s="13"/>
-      <c r="W44" s="13"/>
-      <c r="X44" s="13"/>
-      <c r="Y44" s="13"/>
-    </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V44" s="13">
+        <v>0</v>
+      </c>
+      <c r="W44" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -26692,12 +26786,14 @@
       <c r="U45" s="13">
         <v>0</v>
       </c>
-      <c r="V45" s="13"/>
-      <c r="W45" s="13"/>
-      <c r="X45" s="13"/>
-      <c r="Y45" s="13"/>
-    </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V45" s="13">
+        <v>0</v>
+      </c>
+      <c r="W45" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>19</v>
       </c>
@@ -26761,12 +26857,14 @@
       <c r="U46" s="13">
         <v>0</v>
       </c>
-      <c r="V46" s="13"/>
-      <c r="W46" s="13"/>
-      <c r="X46" s="13"/>
-      <c r="Y46" s="13"/>
-    </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V46" s="13">
+        <v>0</v>
+      </c>
+      <c r="W46" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>20</v>
       </c>
@@ -26830,12 +26928,14 @@
       <c r="U47" s="13">
         <v>0</v>
       </c>
-      <c r="V47" s="13"/>
-      <c r="W47" s="13"/>
-      <c r="X47" s="13"/>
-      <c r="Y47" s="13"/>
-    </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V47" s="13">
+        <v>0</v>
+      </c>
+      <c r="W47" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>74</v>
       </c>
@@ -26899,12 +26999,14 @@
       <c r="U48" s="13">
         <v>0</v>
       </c>
-      <c r="V48" s="13"/>
-      <c r="W48" s="13"/>
-      <c r="X48" s="13"/>
-      <c r="Y48" s="13"/>
-    </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V48" s="13">
+        <v>0</v>
+      </c>
+      <c r="W48" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>75</v>
       </c>
@@ -26968,12 +27070,14 @@
       <c r="U49" s="13">
         <v>0</v>
       </c>
-      <c r="V49" s="13"/>
-      <c r="W49" s="13"/>
-      <c r="X49" s="13"/>
-      <c r="Y49" s="13"/>
-    </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V49" s="13">
+        <v>0</v>
+      </c>
+      <c r="W49" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>21</v>
       </c>
@@ -27037,12 +27141,14 @@
       <c r="U50" s="13">
         <v>0</v>
       </c>
-      <c r="V50" s="13"/>
-      <c r="W50" s="13"/>
-      <c r="X50" s="13"/>
-      <c r="Y50" s="13"/>
-    </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V50" s="13">
+        <v>0</v>
+      </c>
+      <c r="W50" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>97</v>
       </c>
@@ -27106,12 +27212,14 @@
       <c r="U51" s="13">
         <v>0</v>
       </c>
-      <c r="V51" s="13"/>
-      <c r="W51" s="13"/>
-      <c r="X51" s="13"/>
-      <c r="Y51" s="13"/>
-    </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V51" s="13">
+        <v>0</v>
+      </c>
+      <c r="W51" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>103</v>
       </c>
@@ -27175,12 +27283,14 @@
       <c r="U52" s="13">
         <v>0</v>
       </c>
-      <c r="V52" s="13"/>
-      <c r="W52" s="13"/>
-      <c r="X52" s="13"/>
-      <c r="Y52" s="13"/>
-    </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V52" s="13">
+        <v>0</v>
+      </c>
+      <c r="W52" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>104</v>
       </c>
@@ -27244,12 +27354,14 @@
       <c r="U53" s="13">
         <v>0</v>
       </c>
-      <c r="V53" s="13"/>
-      <c r="W53" s="13"/>
-      <c r="X53" s="13"/>
-      <c r="Y53" s="13"/>
-    </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V53" s="13">
+        <v>0</v>
+      </c>
+      <c r="W53" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>105</v>
       </c>
@@ -27313,12 +27425,14 @@
       <c r="U54" s="13">
         <v>0</v>
       </c>
-      <c r="V54" s="13"/>
-      <c r="W54" s="13"/>
-      <c r="X54" s="13"/>
-      <c r="Y54" s="13"/>
-    </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V54" s="13">
+        <v>0</v>
+      </c>
+      <c r="W54" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>106</v>
       </c>
@@ -27382,12 +27496,14 @@
       <c r="U55" s="13">
         <v>0</v>
       </c>
-      <c r="V55" s="13"/>
-      <c r="W55" s="13"/>
-      <c r="X55" s="13"/>
-      <c r="Y55" s="13"/>
-    </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V55" s="13">
+        <v>0</v>
+      </c>
+      <c r="W55" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>124</v>
       </c>
@@ -27451,12 +27567,14 @@
       <c r="U56" s="13">
         <v>0</v>
       </c>
-      <c r="V56" s="13"/>
-      <c r="W56" s="13"/>
-      <c r="X56" s="13"/>
-      <c r="Y56" s="13"/>
-    </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V56" s="13">
+        <v>0</v>
+      </c>
+      <c r="W56" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>125</v>
       </c>
@@ -27520,12 +27638,14 @@
       <c r="U57" s="13">
         <v>0</v>
       </c>
-      <c r="V57" s="13"/>
-      <c r="W57" s="13"/>
-      <c r="X57" s="13"/>
-      <c r="Y57" s="13"/>
-    </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V57" s="13">
+        <v>0</v>
+      </c>
+      <c r="W57" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>123</v>
       </c>
@@ -27589,12 +27709,14 @@
       <c r="U58" s="13">
         <v>3</v>
       </c>
-      <c r="V58" s="13"/>
-      <c r="W58" s="13"/>
-      <c r="X58" s="13"/>
-      <c r="Y58" s="13"/>
-    </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V58" s="13">
+        <v>7</v>
+      </c>
+      <c r="W58" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>126</v>
       </c>
@@ -27658,12 +27780,14 @@
       <c r="U59" s="13">
         <v>3</v>
       </c>
-      <c r="V59" s="13"/>
-      <c r="W59" s="13"/>
-      <c r="X59" s="13"/>
-      <c r="Y59" s="13"/>
-    </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V59" s="13">
+        <v>0</v>
+      </c>
+      <c r="W59" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>127</v>
       </c>
@@ -27727,12 +27851,14 @@
       <c r="U60" s="13">
         <v>3</v>
       </c>
-      <c r="V60" s="13"/>
-      <c r="W60" s="13"/>
-      <c r="X60" s="13"/>
-      <c r="Y60" s="13"/>
-    </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V60" s="13">
+        <v>0</v>
+      </c>
+      <c r="W60" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>128</v>
       </c>
@@ -27796,12 +27922,14 @@
       <c r="U61" s="13">
         <v>3</v>
       </c>
-      <c r="V61" s="13"/>
-      <c r="W61" s="13"/>
-      <c r="X61" s="13"/>
-      <c r="Y61" s="13"/>
-    </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V61" s="13">
+        <v>0</v>
+      </c>
+      <c r="W61" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>129</v>
       </c>
@@ -27865,12 +27993,14 @@
       <c r="U62" s="13">
         <v>2</v>
       </c>
-      <c r="V62" s="13"/>
-      <c r="W62" s="13"/>
-      <c r="X62" s="13"/>
-      <c r="Y62" s="13"/>
-    </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V62" s="13">
+        <v>2</v>
+      </c>
+      <c r="W62" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>130</v>
       </c>
@@ -27934,12 +28064,14 @@
       <c r="U63" s="13">
         <v>2</v>
       </c>
-      <c r="V63" s="13"/>
-      <c r="W63" s="13"/>
-      <c r="X63" s="13"/>
-      <c r="Y63" s="13"/>
-    </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V63" s="13">
+        <v>0</v>
+      </c>
+      <c r="W63" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>131</v>
       </c>
@@ -28003,12 +28135,14 @@
       <c r="U64" s="13">
         <v>2</v>
       </c>
-      <c r="V64" s="13"/>
-      <c r="W64" s="13"/>
-      <c r="X64" s="13"/>
-      <c r="Y64" s="13"/>
-    </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V64" s="13">
+        <v>0</v>
+      </c>
+      <c r="W64" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>132</v>
       </c>
@@ -28072,12 +28206,14 @@
       <c r="U65" s="13">
         <v>3</v>
       </c>
-      <c r="V65" s="13"/>
-      <c r="W65" s="13"/>
-      <c r="X65" s="13"/>
-      <c r="Y65" s="13"/>
-    </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V65" s="13">
+        <v>0</v>
+      </c>
+      <c r="W65" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>133</v>
       </c>
@@ -28141,12 +28277,14 @@
       <c r="U66" s="13">
         <v>3</v>
       </c>
-      <c r="V66" s="13"/>
-      <c r="W66" s="13"/>
-      <c r="X66" s="13"/>
-      <c r="Y66" s="13"/>
-    </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V66" s="13">
+        <v>0</v>
+      </c>
+      <c r="W66" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>134</v>
       </c>
@@ -28210,12 +28348,14 @@
       <c r="U67" s="13">
         <v>3</v>
       </c>
-      <c r="V67" s="13"/>
-      <c r="W67" s="13"/>
-      <c r="X67" s="13"/>
-      <c r="Y67" s="13"/>
-    </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V67" s="13">
+        <v>0</v>
+      </c>
+      <c r="W67" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>135</v>
       </c>
@@ -28279,12 +28419,14 @@
       <c r="U68" s="13">
         <v>3</v>
       </c>
-      <c r="V68" s="13"/>
-      <c r="W68" s="13"/>
-      <c r="X68" s="13"/>
-      <c r="Y68" s="13"/>
-    </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V68" s="13">
+        <v>0</v>
+      </c>
+      <c r="W68" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>136</v>
       </c>
@@ -28348,12 +28490,14 @@
       <c r="U69" s="13">
         <v>3</v>
       </c>
-      <c r="V69" s="13"/>
-      <c r="W69" s="13"/>
-      <c r="X69" s="13"/>
-      <c r="Y69" s="13"/>
-    </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V69" s="13">
+        <v>0</v>
+      </c>
+      <c r="W69" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>137</v>
       </c>
@@ -28417,12 +28561,14 @@
       <c r="U70" s="13">
         <v>3</v>
       </c>
-      <c r="V70" s="13"/>
-      <c r="W70" s="13"/>
-      <c r="X70" s="13"/>
-      <c r="Y70" s="13"/>
-    </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V70" s="13">
+        <v>0</v>
+      </c>
+      <c r="W70" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>138</v>
       </c>
@@ -28486,12 +28632,14 @@
       <c r="U71" s="13">
         <v>3</v>
       </c>
-      <c r="V71" s="13"/>
-      <c r="W71" s="13"/>
-      <c r="X71" s="13"/>
-      <c r="Y71" s="13"/>
-    </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V71" s="13">
+        <v>0</v>
+      </c>
+      <c r="W71" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>139</v>
       </c>
@@ -28555,514 +28703,16 @@
       <c r="U72" s="13">
         <v>2</v>
       </c>
-      <c r="V72" s="13"/>
-      <c r="W72" s="13"/>
-      <c r="X72" s="13"/>
-      <c r="Y72" s="13"/>
-    </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="C74" s="1"/>
-      <c r="D74" s="31"/>
-      <c r="E74" s="13"/>
-      <c r="F74" s="13"/>
-      <c r="G74" s="13"/>
-      <c r="H74" s="13"/>
-      <c r="I74" s="13"/>
-      <c r="J74" s="13"/>
-      <c r="K74" s="13"/>
-      <c r="L74" s="13"/>
-      <c r="M74" s="13"/>
-      <c r="N74" s="13"/>
-      <c r="O74" s="13"/>
-      <c r="P74" s="13"/>
-      <c r="Q74" s="13"/>
-      <c r="R74" s="13"/>
-      <c r="S74" s="13"/>
-      <c r="T74" s="13"/>
-      <c r="U74" s="13"/>
-      <c r="V74" s="13"/>
-      <c r="W74" s="13"/>
-      <c r="X74" s="13"/>
-      <c r="Y74" s="13"/>
-    </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="C75" s="1"/>
-      <c r="D75" s="8"/>
-      <c r="E75" s="13"/>
-      <c r="F75" s="13"/>
-      <c r="G75" s="13"/>
-      <c r="H75" s="13"/>
-      <c r="I75" s="13"/>
-      <c r="J75" s="13"/>
-      <c r="K75" s="13"/>
-      <c r="L75" s="13"/>
-      <c r="M75" s="13"/>
-      <c r="N75" s="13"/>
-      <c r="O75" s="13"/>
-      <c r="P75" s="13"/>
-      <c r="Q75" s="13"/>
-      <c r="R75" s="13"/>
-      <c r="S75" s="13"/>
-      <c r="T75" s="13"/>
-      <c r="U75" s="13"/>
-      <c r="V75" s="13"/>
-      <c r="W75" s="13"/>
-      <c r="X75" s="13"/>
-      <c r="Y75" s="13"/>
-    </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="C76" s="1"/>
-      <c r="D76" s="8"/>
-      <c r="E76" s="13"/>
-      <c r="F76" s="13"/>
-      <c r="G76" s="13"/>
-      <c r="H76" s="13"/>
-      <c r="I76" s="13"/>
-      <c r="J76" s="13"/>
-      <c r="K76" s="13"/>
-      <c r="L76" s="13"/>
-      <c r="M76" s="13"/>
-      <c r="N76" s="13"/>
-      <c r="O76" s="13"/>
-      <c r="P76" s="13"/>
-      <c r="Q76" s="13"/>
-      <c r="R76" s="13"/>
-      <c r="S76" s="13"/>
-      <c r="T76" s="13"/>
-      <c r="U76" s="13"/>
-      <c r="V76" s="13"/>
-      <c r="W76" s="13"/>
-      <c r="X76" s="13"/>
-      <c r="Y76" s="13"/>
-    </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="C77" s="1"/>
-      <c r="D77" s="8"/>
-      <c r="E77" s="13"/>
-      <c r="F77" s="13"/>
-      <c r="G77" s="13"/>
-      <c r="H77" s="13"/>
-      <c r="I77" s="13"/>
-      <c r="J77" s="13"/>
-      <c r="K77" s="13"/>
-      <c r="L77" s="13"/>
-      <c r="M77" s="13"/>
-      <c r="N77" s="13"/>
-      <c r="O77" s="13"/>
-      <c r="P77" s="13"/>
-      <c r="Q77" s="13"/>
-      <c r="R77" s="13"/>
-      <c r="S77" s="13"/>
-      <c r="T77" s="13"/>
-      <c r="U77" s="13"/>
-      <c r="V77" s="13"/>
-      <c r="W77" s="13"/>
-      <c r="X77" s="13"/>
-      <c r="Y77" s="13"/>
-    </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="C78" s="1"/>
-      <c r="D78" s="8"/>
-      <c r="E78" s="13"/>
-      <c r="F78" s="13"/>
-      <c r="G78" s="13"/>
-      <c r="H78" s="13"/>
-      <c r="I78" s="13"/>
-      <c r="J78" s="13"/>
-      <c r="K78" s="13"/>
-      <c r="L78" s="13"/>
-      <c r="M78" s="13"/>
-      <c r="N78" s="13"/>
-      <c r="O78" s="13"/>
-      <c r="P78" s="13"/>
-      <c r="Q78" s="13"/>
-      <c r="R78" s="13"/>
-      <c r="S78" s="13"/>
-      <c r="T78" s="13"/>
-      <c r="U78" s="13"/>
-      <c r="V78" s="13"/>
-      <c r="W78" s="13"/>
-      <c r="X78" s="13"/>
-      <c r="Y78" s="13"/>
-    </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="C79" s="1"/>
-      <c r="D79" s="8"/>
-      <c r="E79" s="13"/>
-      <c r="F79" s="13"/>
-      <c r="G79" s="13"/>
-      <c r="H79" s="13"/>
-      <c r="I79" s="13"/>
-      <c r="J79" s="13"/>
-      <c r="K79" s="13"/>
-      <c r="L79" s="13"/>
-      <c r="M79" s="13"/>
-      <c r="N79" s="13"/>
-      <c r="O79" s="13"/>
-      <c r="P79" s="13"/>
-      <c r="Q79" s="13"/>
-      <c r="R79" s="13"/>
-      <c r="S79" s="13"/>
-      <c r="T79" s="13"/>
-      <c r="U79" s="13"/>
-      <c r="V79" s="13"/>
-      <c r="W79" s="13"/>
-      <c r="X79" s="13"/>
-      <c r="Y79" s="13"/>
-    </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="C80" s="1"/>
-      <c r="D80" s="8"/>
-      <c r="E80" s="13"/>
-      <c r="F80" s="13"/>
-      <c r="G80" s="13"/>
-      <c r="H80" s="13"/>
-      <c r="I80" s="13"/>
-      <c r="J80" s="13"/>
-      <c r="K80" s="13"/>
-      <c r="L80" s="13"/>
-      <c r="M80" s="13"/>
-      <c r="N80" s="13"/>
-      <c r="O80" s="13"/>
-      <c r="P80" s="13"/>
-      <c r="Q80" s="13"/>
-      <c r="R80" s="13"/>
-      <c r="S80" s="13"/>
-      <c r="T80" s="13"/>
-      <c r="U80" s="13"/>
-      <c r="V80" s="13"/>
-      <c r="W80" s="13"/>
-      <c r="X80" s="13"/>
-      <c r="Y80" s="13"/>
-    </row>
-    <row r="81" spans="3:25" x14ac:dyDescent="0.3">
-      <c r="C81" s="1"/>
-      <c r="D81" s="8"/>
-      <c r="E81" s="13"/>
-      <c r="F81" s="13"/>
-      <c r="G81" s="13"/>
-      <c r="H81" s="13"/>
-      <c r="I81" s="13"/>
-      <c r="J81" s="13"/>
-      <c r="K81" s="13"/>
-      <c r="L81" s="13"/>
-      <c r="M81" s="13"/>
-      <c r="N81" s="13"/>
-      <c r="O81" s="13"/>
-      <c r="P81" s="13"/>
-      <c r="Q81" s="13"/>
-      <c r="R81" s="13"/>
-      <c r="S81" s="13"/>
-      <c r="T81" s="13"/>
-      <c r="U81" s="13"/>
-      <c r="V81" s="13"/>
-      <c r="W81" s="13"/>
-      <c r="X81" s="13"/>
-      <c r="Y81" s="13"/>
-    </row>
-    <row r="82" spans="3:25" x14ac:dyDescent="0.3">
-      <c r="C82" s="1"/>
-      <c r="D82" s="8"/>
-      <c r="E82" s="13"/>
-      <c r="F82" s="13"/>
-      <c r="G82" s="13"/>
-      <c r="H82" s="13"/>
-      <c r="I82" s="13"/>
-      <c r="J82" s="13"/>
-      <c r="K82" s="13"/>
-      <c r="L82" s="13"/>
-      <c r="M82" s="13"/>
-      <c r="N82" s="13"/>
-      <c r="O82" s="13"/>
-      <c r="P82" s="13"/>
-      <c r="Q82" s="13"/>
-      <c r="R82" s="13"/>
-      <c r="S82" s="13"/>
-      <c r="T82" s="13"/>
-      <c r="U82" s="13"/>
-      <c r="V82" s="13"/>
-      <c r="W82" s="13"/>
-      <c r="X82" s="13"/>
-      <c r="Y82" s="13"/>
-    </row>
-    <row r="83" spans="3:25" x14ac:dyDescent="0.3">
-      <c r="C83" s="1"/>
-      <c r="D83" s="8"/>
-      <c r="E83" s="13"/>
-      <c r="F83" s="13"/>
-      <c r="G83" s="13"/>
-      <c r="H83" s="13"/>
-      <c r="I83" s="13"/>
-      <c r="J83" s="13"/>
-      <c r="K83" s="13"/>
-      <c r="L83" s="13"/>
-      <c r="M83" s="13"/>
-      <c r="N83" s="13"/>
-      <c r="O83" s="13"/>
-      <c r="P83" s="13"/>
-      <c r="Q83" s="13"/>
-      <c r="R83" s="13"/>
-      <c r="S83" s="13"/>
-      <c r="T83" s="13"/>
-      <c r="U83" s="13"/>
-      <c r="V83" s="13"/>
-      <c r="W83" s="13"/>
-      <c r="X83" s="13"/>
-      <c r="Y83" s="13"/>
-    </row>
-    <row r="84" spans="3:25" x14ac:dyDescent="0.3">
-      <c r="C84" s="1"/>
-      <c r="D84" s="8"/>
-      <c r="E84" s="13"/>
-      <c r="F84" s="13"/>
-      <c r="G84" s="13"/>
-      <c r="H84" s="13"/>
-      <c r="I84" s="13"/>
-      <c r="J84" s="13"/>
-      <c r="K84" s="13"/>
-      <c r="L84" s="13"/>
-      <c r="M84" s="13"/>
-      <c r="N84" s="13"/>
-      <c r="O84" s="13"/>
-      <c r="P84" s="13"/>
-      <c r="Q84" s="13"/>
-      <c r="R84" s="13"/>
-      <c r="S84" s="13"/>
-      <c r="T84" s="13"/>
-      <c r="U84" s="13"/>
-      <c r="V84" s="13"/>
-      <c r="W84" s="13"/>
-      <c r="X84" s="13"/>
-      <c r="Y84" s="13"/>
-    </row>
-    <row r="85" spans="3:25" x14ac:dyDescent="0.3">
-      <c r="C85" s="1"/>
-      <c r="D85" s="8"/>
-      <c r="E85" s="13"/>
-      <c r="F85" s="13"/>
-      <c r="G85" s="13"/>
-      <c r="H85" s="13"/>
-      <c r="I85" s="13"/>
-      <c r="J85" s="13"/>
-      <c r="K85" s="13"/>
-      <c r="L85" s="13"/>
-      <c r="M85" s="13"/>
-      <c r="N85" s="13"/>
-      <c r="O85" s="13"/>
-      <c r="P85" s="13"/>
-      <c r="Q85" s="13"/>
-      <c r="R85" s="13"/>
-      <c r="S85" s="13"/>
-      <c r="T85" s="13"/>
-      <c r="U85" s="13"/>
-      <c r="V85" s="13"/>
-      <c r="W85" s="13"/>
-      <c r="X85" s="13"/>
-      <c r="Y85" s="13"/>
-    </row>
-    <row r="86" spans="3:25" x14ac:dyDescent="0.3">
-      <c r="C86" s="1"/>
-      <c r="D86" s="8"/>
-      <c r="E86" s="13"/>
-      <c r="F86" s="13"/>
-      <c r="G86" s="13"/>
-      <c r="H86" s="13"/>
-      <c r="I86" s="13"/>
-      <c r="J86" s="13"/>
-      <c r="K86" s="13"/>
-      <c r="L86" s="13"/>
-      <c r="M86" s="13"/>
-      <c r="N86" s="13"/>
-      <c r="O86" s="13"/>
-      <c r="P86" s="13"/>
-      <c r="Q86" s="13"/>
-      <c r="R86" s="13"/>
-      <c r="S86" s="13"/>
-      <c r="T86" s="13"/>
-      <c r="U86" s="13"/>
-      <c r="V86" s="13"/>
-      <c r="W86" s="13"/>
-      <c r="X86" s="13"/>
-      <c r="Y86" s="13"/>
-    </row>
-    <row r="87" spans="3:25" x14ac:dyDescent="0.3">
-      <c r="C87" s="1"/>
-      <c r="D87" s="8"/>
-      <c r="E87" s="13"/>
-      <c r="F87" s="13"/>
-      <c r="G87" s="13"/>
-      <c r="H87" s="13"/>
-      <c r="I87" s="13"/>
-      <c r="J87" s="13"/>
-      <c r="K87" s="13"/>
-      <c r="L87" s="13"/>
-      <c r="M87" s="13"/>
-      <c r="N87" s="13"/>
-      <c r="O87" s="13"/>
-      <c r="P87" s="13"/>
-      <c r="Q87" s="13"/>
-      <c r="R87" s="13"/>
-      <c r="S87" s="13"/>
-      <c r="T87" s="13"/>
-      <c r="U87" s="13"/>
-      <c r="V87" s="13"/>
-      <c r="W87" s="13"/>
-      <c r="X87" s="13"/>
-      <c r="Y87" s="13"/>
-    </row>
-    <row r="88" spans="3:25" x14ac:dyDescent="0.3">
-      <c r="C88" s="1"/>
-      <c r="D88" s="8"/>
-      <c r="E88" s="13"/>
-      <c r="F88" s="13"/>
-      <c r="G88" s="13"/>
-      <c r="H88" s="13"/>
-      <c r="I88" s="13"/>
-      <c r="J88" s="13"/>
-      <c r="K88" s="13"/>
-      <c r="L88" s="13"/>
-      <c r="M88" s="13"/>
-      <c r="N88" s="13"/>
-      <c r="O88" s="13"/>
-      <c r="P88" s="13"/>
-      <c r="Q88" s="13"/>
-      <c r="R88" s="13"/>
-      <c r="S88" s="13"/>
-      <c r="T88" s="13"/>
-      <c r="U88" s="13"/>
-      <c r="V88" s="13"/>
-      <c r="W88" s="13"/>
-      <c r="X88" s="13"/>
-      <c r="Y88" s="13"/>
-    </row>
-    <row r="89" spans="3:25" x14ac:dyDescent="0.3">
-      <c r="C89" s="1"/>
-      <c r="D89" s="8"/>
-      <c r="E89" s="13"/>
-      <c r="F89" s="13"/>
-      <c r="G89" s="13"/>
-      <c r="H89" s="13"/>
-      <c r="I89" s="13"/>
-      <c r="J89" s="13"/>
-      <c r="K89" s="13"/>
-      <c r="L89" s="13"/>
-      <c r="M89" s="13"/>
-      <c r="N89" s="13"/>
-      <c r="O89" s="13"/>
-      <c r="P89" s="13"/>
-      <c r="Q89" s="13"/>
-      <c r="R89" s="13"/>
-      <c r="S89" s="13"/>
-      <c r="T89" s="13"/>
-      <c r="U89" s="13"/>
-      <c r="V89" s="13"/>
-      <c r="W89" s="13"/>
-      <c r="X89" s="13"/>
-      <c r="Y89" s="13"/>
-    </row>
-    <row r="90" spans="3:25" x14ac:dyDescent="0.3">
-      <c r="C90" s="1"/>
-      <c r="D90" s="8"/>
-      <c r="E90" s="13"/>
-      <c r="F90" s="13"/>
-      <c r="G90" s="13"/>
-      <c r="H90" s="13"/>
-      <c r="I90" s="13"/>
-      <c r="J90" s="13"/>
-      <c r="K90" s="13"/>
-      <c r="L90" s="13"/>
-      <c r="M90" s="13"/>
-      <c r="N90" s="13"/>
-      <c r="O90" s="13"/>
-      <c r="P90" s="13"/>
-      <c r="Q90" s="13"/>
-      <c r="R90" s="13"/>
-      <c r="S90" s="13"/>
-      <c r="T90" s="13"/>
-      <c r="U90" s="13"/>
-      <c r="V90" s="13"/>
-      <c r="W90" s="13"/>
-      <c r="X90" s="13"/>
-      <c r="Y90" s="13"/>
-    </row>
-    <row r="91" spans="3:25" x14ac:dyDescent="0.3">
-      <c r="C91" s="1"/>
-      <c r="D91" s="8"/>
-      <c r="E91" s="13"/>
-      <c r="F91" s="13"/>
-      <c r="G91" s="13"/>
-      <c r="H91" s="13"/>
-      <c r="I91" s="13"/>
-      <c r="J91" s="13"/>
-      <c r="K91" s="13"/>
-      <c r="L91" s="13"/>
-      <c r="M91" s="13"/>
-      <c r="N91" s="13"/>
-      <c r="O91" s="13"/>
-      <c r="P91" s="13"/>
-      <c r="Q91" s="13"/>
-      <c r="R91" s="13"/>
-      <c r="S91" s="13"/>
-      <c r="T91" s="13"/>
-      <c r="U91" s="13"/>
-      <c r="V91" s="13"/>
-      <c r="W91" s="13"/>
-      <c r="X91" s="13"/>
-      <c r="Y91" s="13"/>
-    </row>
-    <row r="92" spans="3:25" x14ac:dyDescent="0.3">
-      <c r="C92" s="1"/>
-      <c r="D92" s="8"/>
-      <c r="E92" s="13"/>
-      <c r="F92" s="13"/>
-      <c r="G92" s="13"/>
-      <c r="H92" s="13"/>
-      <c r="I92" s="13"/>
-      <c r="J92" s="13"/>
-      <c r="K92" s="13"/>
-      <c r="L92" s="13"/>
-      <c r="M92" s="13"/>
-      <c r="N92" s="13"/>
-      <c r="O92" s="13"/>
-      <c r="P92" s="13"/>
-      <c r="Q92" s="13"/>
-      <c r="R92" s="13"/>
-      <c r="S92" s="13"/>
-      <c r="T92" s="13"/>
-      <c r="U92" s="13"/>
-      <c r="V92" s="13"/>
-      <c r="W92" s="13"/>
-      <c r="X92" s="13"/>
-      <c r="Y92" s="13"/>
-    </row>
-    <row r="93" spans="3:25" x14ac:dyDescent="0.3">
-      <c r="C93" s="1"/>
-      <c r="D93" s="8"/>
-      <c r="E93" s="13"/>
-      <c r="F93" s="13"/>
-      <c r="G93" s="13"/>
-      <c r="H93" s="13"/>
-      <c r="I93" s="13"/>
-      <c r="J93" s="13"/>
-      <c r="K93" s="13"/>
-      <c r="L93" s="13"/>
-      <c r="M93" s="13"/>
-      <c r="N93" s="13"/>
-      <c r="O93" s="13"/>
-      <c r="P93" s="13"/>
-      <c r="Q93" s="13"/>
-      <c r="R93" s="13"/>
-      <c r="S93" s="13"/>
-      <c r="T93" s="13"/>
-      <c r="U93" s="13"/>
-      <c r="V93" s="13"/>
-      <c r="W93" s="13"/>
-      <c r="X93" s="13"/>
-      <c r="Y93" s="13"/>
+      <c r="V72" s="13">
+        <v>0</v>
+      </c>
+      <c r="W72" s="13">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
-  <conditionalFormatting sqref="A1:D29 E1:Y1">
+  <conditionalFormatting sqref="A1:D29 E1:W1">
     <cfRule type="beginsWith" dxfId="14" priority="59" operator="beginsWith" text="es">
       <formula>LEFT(A1,LEN("es"))="es"</formula>
     </cfRule>
@@ -29078,7 +28728,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B74:B93 B31:B72">
+  <conditionalFormatting sqref="B31:B72">
     <cfRule type="cellIs" dxfId="10" priority="237" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
@@ -29086,7 +28736,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D74:D93 D31:D72">
+  <conditionalFormatting sqref="D31:D72">
     <cfRule type="cellIs" dxfId="5" priority="310" operator="equal">
       <formula>2</formula>
     </cfRule>
@@ -29094,7 +28744,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:Y1 A1:D29">
+  <conditionalFormatting sqref="E1:W1 A1:D29">
     <cfRule type="beginsWith" dxfId="3" priority="60" operator="beginsWith" text="de">
       <formula>LEFT(A1,LEN("de"))="de"</formula>
     </cfRule>
@@ -29102,12 +28752,12 @@
       <formula>NOT(ISERROR(SEARCH("trade",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E31:Y32 E74:Y93 E34:Y72">
+  <conditionalFormatting sqref="E31:W32 E34:W72">
     <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E74:Y93 E31:Y72">
+  <conditionalFormatting sqref="E31:W72">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
@@ -29149,7 +28799,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>B74:B93 B31:B72</xm:sqref>
+          <xm:sqref>B31:B72</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -29159,10 +28809,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49CB70FA-B08B-40E6-A846-223D7188DBF8}">
-  <dimension ref="A1:B247"/>
+  <dimension ref="A1:B223"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="F79" sqref="F79"/>
+    <sheetView topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82:XFD105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30324,78 +29974,6 @@
     <row r="223" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A223" s="28"/>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A224" s="28"/>
-    </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A225" s="28"/>
-    </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A226" s="28"/>
-    </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A227" s="28"/>
-    </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A228" s="28"/>
-    </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A229" s="28"/>
-    </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A230" s="28"/>
-    </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A231" s="28"/>
-    </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A232" s="28"/>
-    </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A233" s="28"/>
-    </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A234" s="28"/>
-    </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A235" s="28"/>
-    </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A236" s="28"/>
-    </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A237" s="28"/>
-    </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A238" s="28"/>
-    </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A239" s="28"/>
-    </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A240" s="28"/>
-    </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A241" s="28"/>
-    </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A242" s="28"/>
-    </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A243" s="28"/>
-    </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A244" s="28"/>
-    </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A245" s="28"/>
-    </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A246" s="28"/>
-    </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A247" s="28"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -30403,10 +29981,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EE798E0-AE48-44C7-A092-F3DD5857D33D}">
-  <dimension ref="A1:Q247"/>
+  <dimension ref="A1:Q243"/>
   <sheetViews>
-    <sheetView topLeftCell="A221" workbookViewId="0">
-      <selection activeCell="A242" sqref="A239:A243"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -43196,18 +42774,6 @@
       <c r="Q243">
         <v>105</v>
       </c>
-    </row>
-    <row r="244" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A244" s="28"/>
-    </row>
-    <row r="245" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A245" s="28"/>
-    </row>
-    <row r="246" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A246" s="28"/>
-    </row>
-    <row r="247" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A247" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>